<commit_message>
Made final touches to the Association
</commit_message>
<xml_diff>
--- a/original_files/GULU PWDs.xlsx
+++ b/original_files/GULU PWDs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="145">
   <si>
     <t>S/N</t>
   </si>
@@ -447,13 +447,25 @@
   </si>
   <si>
     <t>AUMA SANTA</t>
+  </si>
+  <si>
+    <t>UNION</t>
+  </si>
+  <si>
+    <t>LALOGI SUBCOUNTY PARISH DISABILITY UNION</t>
+  </si>
+  <si>
+    <t>LAKWANA SUB COUNTY PARISH UNION</t>
+  </si>
+  <si>
+    <t>LABORA SUBCOUNTY PARISH UNION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,6 +476,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -527,43 +547,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,9 +879,10 @@
     <col min="5" max="5" width="27.7109375" customWidth="1"/>
     <col min="6" max="6" width="31.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="8" max="8" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -882,8 +904,11 @@
       <c r="G1" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H1" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -905,8 +930,11 @@
       <c r="G2" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H2" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -928,8 +956,11 @@
       <c r="G3" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H3" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -951,8 +982,11 @@
       <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H4" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -974,8 +1008,11 @@
       <c r="G5" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H5" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -997,8 +1034,11 @@
       <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H6" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1020,8 +1060,11 @@
       <c r="G7" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H7" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1043,8 +1086,11 @@
       <c r="G8" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H8" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1064,8 +1110,11 @@
       <c r="G9" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H9" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1087,8 +1136,11 @@
       <c r="G10" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H10" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1110,8 +1162,11 @@
       <c r="G11" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H11" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1133,8 +1188,11 @@
       <c r="G12" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H12" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1156,8 +1214,11 @@
       <c r="G13" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H13" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1177,8 +1238,11 @@
       <c r="G14" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H14" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1200,8 +1264,11 @@
       <c r="G15" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H15" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1223,8 +1290,11 @@
       <c r="G16" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H16" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1246,8 +1316,11 @@
       <c r="G17" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H17" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1269,8 +1342,11 @@
       <c r="G18" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H18" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1290,8 +1366,11 @@
       <c r="G19" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H19" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1313,8 +1392,11 @@
       <c r="G20" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H20" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1334,8 +1416,11 @@
       <c r="G21" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H21" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1355,8 +1440,11 @@
       <c r="G22" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H22" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1376,8 +1464,11 @@
       <c r="G23" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H23" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -1399,8 +1490,11 @@
       <c r="G24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H24" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -1420,8 +1514,11 @@
       <c r="G25" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H25" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>25</v>
       </c>
@@ -1441,8 +1538,11 @@
       <c r="G26" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H26" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -1464,8 +1564,11 @@
       <c r="G27" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H27" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -1485,8 +1588,11 @@
       <c r="G28" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H28" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -1506,8 +1612,11 @@
       <c r="G29" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H29" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -1527,8 +1636,11 @@
       <c r="G30" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H30" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -1548,8 +1660,11 @@
       <c r="G31" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H31" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -1571,8 +1686,11 @@
       <c r="G32" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H32" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>32</v>
       </c>
@@ -1594,8 +1712,11 @@
       <c r="G33" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H33" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>33</v>
       </c>
@@ -1617,8 +1738,11 @@
       <c r="G34" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H34" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>34</v>
       </c>
@@ -1640,8 +1764,11 @@
       <c r="G35" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H35" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>35</v>
       </c>
@@ -1663,8 +1790,11 @@
       <c r="G36" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H36" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>36</v>
       </c>
@@ -1684,8 +1814,11 @@
       <c r="G37" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H37" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>37</v>
       </c>
@@ -1707,8 +1840,11 @@
       <c r="G38" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H38" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>38</v>
       </c>
@@ -1730,8 +1866,11 @@
       <c r="G39" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H39" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>39</v>
       </c>
@@ -1753,8 +1892,11 @@
       <c r="G40" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H40" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>40</v>
       </c>
@@ -1774,8 +1916,11 @@
       <c r="G41" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H41" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>41</v>
       </c>
@@ -1797,8 +1942,11 @@
       <c r="G42" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H42" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>42</v>
       </c>
@@ -1820,8 +1968,11 @@
       <c r="G43" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H43" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>43</v>
       </c>
@@ -1843,8 +1994,11 @@
       <c r="G44" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H44" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>44</v>
       </c>
@@ -1866,8 +2020,11 @@
       <c r="G45" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H45" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>45</v>
       </c>
@@ -1887,8 +2044,11 @@
       <c r="G46" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H46" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>46</v>
       </c>
@@ -1908,8 +2068,11 @@
       <c r="G47" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H47" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>47</v>
       </c>
@@ -1931,8 +2094,11 @@
       <c r="G48" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H48" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>48</v>
       </c>
@@ -1954,8 +2120,11 @@
       <c r="G49" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H49" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>49</v>
       </c>
@@ -1977,8 +2146,11 @@
       <c r="G50" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H50" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>50</v>
       </c>
@@ -1998,8 +2170,11 @@
       <c r="G51" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H51" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>51</v>
       </c>
@@ -2021,8 +2196,11 @@
       <c r="G52" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H52" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>52</v>
       </c>
@@ -2042,8 +2220,11 @@
       <c r="G53" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H53" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>53</v>
       </c>
@@ -2065,8 +2246,11 @@
       <c r="G54" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H54" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>54</v>
       </c>
@@ -2088,8 +2272,11 @@
       <c r="G55" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H55" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>55</v>
       </c>
@@ -2111,8 +2298,11 @@
       <c r="G56" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H56" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>56</v>
       </c>
@@ -2134,8 +2324,11 @@
       <c r="G57" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H57" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>57</v>
       </c>
@@ -2157,8 +2350,11 @@
       <c r="G58" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H58" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>58</v>
       </c>
@@ -2180,8 +2376,11 @@
       <c r="G59" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H59" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>59</v>
       </c>
@@ -2203,8 +2402,11 @@
       <c r="G60" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H60" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>60</v>
       </c>
@@ -2226,8 +2428,11 @@
       <c r="G61" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H61" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>61</v>
       </c>
@@ -2249,8 +2454,11 @@
       <c r="G62" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H62" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>62</v>
       </c>
@@ -2272,8 +2480,11 @@
       <c r="G63" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H63" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>63</v>
       </c>
@@ -2295,8 +2506,11 @@
       <c r="G64" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H64" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>64</v>
       </c>
@@ -2318,8 +2532,11 @@
       <c r="G65" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H65" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>65</v>
       </c>
@@ -2339,8 +2556,11 @@
       <c r="G66" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H66" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>66</v>
       </c>
@@ -2362,8 +2582,11 @@
       <c r="G67" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H67" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>67</v>
       </c>
@@ -2385,8 +2608,11 @@
       <c r="G68" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H68" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>68</v>
       </c>
@@ -2406,8 +2632,11 @@
       <c r="G69" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H69" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>69</v>
       </c>
@@ -2429,8 +2658,11 @@
       <c r="G70" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H70" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>70</v>
       </c>
@@ -2452,8 +2684,11 @@
       <c r="G71" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H71" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>71</v>
       </c>
@@ -2475,8 +2710,11 @@
       <c r="G72" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H72" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>72</v>
       </c>
@@ -2498,8 +2736,11 @@
       <c r="G73" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H73" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>73</v>
       </c>
@@ -2521,8 +2762,11 @@
       <c r="G74" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H74" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>74</v>
       </c>
@@ -2544,8 +2788,11 @@
       <c r="G75" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H75" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>75</v>
       </c>
@@ -2567,8 +2814,11 @@
       <c r="G76" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H76" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>76</v>
       </c>
@@ -2590,8 +2840,11 @@
       <c r="G77" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H77" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>77</v>
       </c>
@@ -2613,8 +2866,11 @@
       <c r="G78" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H78" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>78</v>
       </c>
@@ -2636,8 +2892,11 @@
       <c r="G79" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H79" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>79</v>
       </c>
@@ -2659,8 +2918,11 @@
       <c r="G80" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H80" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>80</v>
       </c>
@@ -2682,8 +2944,11 @@
       <c r="G81" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H81" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>81</v>
       </c>
@@ -2705,8 +2970,11 @@
       <c r="G82" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H82" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>82</v>
       </c>
@@ -2728,8 +2996,11 @@
       <c r="G83" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H83" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>83</v>
       </c>
@@ -2751,8 +3022,11 @@
       <c r="G84" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H84" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>84</v>
       </c>
@@ -2774,8 +3048,11 @@
       <c r="G85" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H85" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>85</v>
       </c>
@@ -2797,8 +3074,11 @@
       <c r="G86" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H86" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>86</v>
       </c>
@@ -2820,8 +3100,11 @@
       <c r="G87" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H87" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>87</v>
       </c>
@@ -2843,8 +3126,11 @@
       <c r="G88" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H88" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>88</v>
       </c>
@@ -2866,8 +3152,11 @@
       <c r="G89" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H89" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>89</v>
       </c>
@@ -2889,8 +3178,11 @@
       <c r="G90" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H90" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>90</v>
       </c>
@@ -2912,8 +3204,11 @@
       <c r="G91" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H91" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>91</v>
       </c>
@@ -2935,8 +3230,11 @@
       <c r="G92" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H92" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>92</v>
       </c>
@@ -2958,8 +3256,11 @@
       <c r="G93" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H93" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <v>93</v>
       </c>
@@ -2981,8 +3282,11 @@
       <c r="G94" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H94" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>94</v>
       </c>
@@ -3004,8 +3308,11 @@
       <c r="G95" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H95" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>95</v>
       </c>
@@ -3026,6 +3333,9 @@
       </c>
       <c r="G96" s="2" t="s">
         <v>127</v>
+      </c>
+      <c r="H96" s="14" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>